<commit_message>
product string to json
</commit_message>
<xml_diff>
--- a/public/temp/user_details.xlsx
+++ b/public/temp/user_details.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="35">
   <si>
     <t>First Name</t>
   </si>
@@ -70,13 +70,19 @@
     <t>america</t>
   </si>
   <si>
-    <t>Protein Shake</t>
+    <t>Chia Seeds</t>
   </si>
   <si>
-    <t>Greek Yoghurt</t>
+    <t>Creatine</t>
   </si>
   <si>
-    <t>Muscle Mass gainer</t>
+    <t>Almond Butter</t>
+  </si>
+  <si>
+    <t>Energy Bar</t>
+  </si>
+  <si>
+    <t>Muscle Mass Gainer</t>
   </si>
   <si>
     <t>Parth</t>
@@ -100,28 +106,16 @@
     <t>India</t>
   </si>
   <si>
-    <t>Peanut butter</t>
+    <t>pranav</t>
   </si>
   <si>
-    <t>Glutamine</t>
+    <t>khandare</t>
   </si>
   <si>
-    <t>Fish Oil</t>
+    <t>pk@gmail.com</t>
   </si>
   <si>
-    <t>Oats</t>
-  </si>
-  <si>
-    <t>Rajasjri</t>
-  </si>
-  <si>
-    <t>राजश्री</t>
-  </si>
-  <si>
-    <t>Etgdfg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Navi Mumbai </t>
+    <t>Thane</t>
   </si>
 </sst>
 </file>
@@ -498,7 +492,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L47"/>
+  <dimension ref="A1:L80"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -655,16 +649,16 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="D5">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E5">
         <v>163</v>
@@ -673,19 +667,19 @@
         <v>56</v>
       </c>
       <c r="G5" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="H5" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="I5" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="J5" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="K5">
-        <v>663082682</v>
+        <v>91231233</v>
       </c>
       <c r="L5" t="s">
         <v>20</v>
@@ -693,54 +687,54 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6">
+        <v>18</v>
+      </c>
+      <c r="E6">
+        <v>163</v>
+      </c>
+      <c r="F6">
+        <v>56</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6">
+        <v>91231233</v>
+      </c>
+      <c r="L6" t="s">
         <v>22</v>
-      </c>
-      <c r="B6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6">
-        <v>20</v>
-      </c>
-      <c r="E6">
-        <v>163</v>
-      </c>
-      <c r="F6">
-        <v>56</v>
-      </c>
-      <c r="G6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" t="s">
-        <v>26</v>
-      </c>
-      <c r="I6" t="s">
-        <v>27</v>
-      </c>
-      <c r="J6" t="s">
-        <v>28</v>
-      </c>
-      <c r="K6">
-        <v>663082682</v>
-      </c>
-      <c r="L6" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="D7">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E7">
         <v>163</v>
@@ -749,74 +743,74 @@
         <v>56</v>
       </c>
       <c r="G7" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="H7" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="I7" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="J7" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="K7">
-        <v>663082682</v>
+        <v>91231233</v>
       </c>
       <c r="L7" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8">
+        <v>18</v>
+      </c>
+      <c r="E8">
+        <v>163</v>
+      </c>
+      <c r="F8">
+        <v>56</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8">
+        <v>91231233</v>
+      </c>
+      <c r="L8" t="s">
         <v>22</v>
-      </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8">
-        <v>20</v>
-      </c>
-      <c r="E8">
-        <v>163</v>
-      </c>
-      <c r="F8">
-        <v>56</v>
-      </c>
-      <c r="G8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I8" t="s">
-        <v>27</v>
-      </c>
-      <c r="J8" t="s">
-        <v>28</v>
-      </c>
-      <c r="K8">
-        <v>663082682</v>
-      </c>
-      <c r="L8" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="D9">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E9">
         <v>163</v>
@@ -825,22 +819,22 @@
         <v>56</v>
       </c>
       <c r="G9" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="H9" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="I9" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="J9" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="K9">
-        <v>663082682</v>
+        <v>91231233</v>
       </c>
       <c r="L9" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -878,7 +872,7 @@
         <v>91231233</v>
       </c>
       <c r="L10" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -916,7 +910,7 @@
         <v>91231233</v>
       </c>
       <c r="L11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -954,7 +948,7 @@
         <v>91231233</v>
       </c>
       <c r="L12" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -992,7 +986,7 @@
         <v>91231233</v>
       </c>
       <c r="L13" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1068,7 +1062,7 @@
         <v>91231233</v>
       </c>
       <c r="L15" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1106,21 +1100,21 @@
         <v>91231233</v>
       </c>
       <c r="L16" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D17">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E17">
         <v>163</v>
@@ -1129,36 +1123,36 @@
         <v>56</v>
       </c>
       <c r="G17" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="H17" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="I17" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="J17" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="K17">
-        <v>91231233</v>
+        <v>663082682</v>
       </c>
       <c r="L17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D18">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E18">
         <v>163</v>
@@ -1167,36 +1161,36 @@
         <v>56</v>
       </c>
       <c r="G18" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="H18" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="I18" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="J18" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="K18">
-        <v>91231233</v>
+        <v>663082682</v>
       </c>
       <c r="L18" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C19" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D19">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E19">
         <v>163</v>
@@ -1205,36 +1199,36 @@
         <v>56</v>
       </c>
       <c r="G19" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="H19" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="I19" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="J19" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="K19">
-        <v>91231233</v>
+        <v>663082682</v>
       </c>
       <c r="L19" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D20">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E20">
         <v>163</v>
@@ -1243,36 +1237,36 @@
         <v>56</v>
       </c>
       <c r="G20" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="H20" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="I20" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="J20" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="K20">
-        <v>91231233</v>
+        <v>663082682</v>
       </c>
       <c r="L20" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D21">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E21">
         <v>163</v>
@@ -1281,36 +1275,36 @@
         <v>56</v>
       </c>
       <c r="G21" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="H21" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="I21" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="J21" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="K21">
-        <v>91231233</v>
+        <v>663082682</v>
       </c>
       <c r="L21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D22">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E22">
         <v>163</v>
@@ -1319,36 +1313,36 @@
         <v>56</v>
       </c>
       <c r="G22" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="H22" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="I22" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="J22" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="K22">
-        <v>91231233</v>
+        <v>663082682</v>
       </c>
       <c r="L22" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D23">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E23">
         <v>163</v>
@@ -1357,19 +1351,19 @@
         <v>56</v>
       </c>
       <c r="G23" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="H23" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="I23" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="J23" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="K23">
-        <v>91231233</v>
+        <v>663082682</v>
       </c>
       <c r="L23" t="s">
         <v>19</v>
@@ -1377,16 +1371,16 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D24">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E24">
         <v>163</v>
@@ -1395,36 +1389,36 @@
         <v>56</v>
       </c>
       <c r="G24" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="H24" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="I24" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="J24" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="K24">
-        <v>91231233</v>
+        <v>663082682</v>
       </c>
       <c r="L24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C25" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D25">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E25">
         <v>163</v>
@@ -1433,36 +1427,36 @@
         <v>56</v>
       </c>
       <c r="G25" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="H25" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="I25" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="J25" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="K25">
-        <v>91231233</v>
+        <v>663082682</v>
       </c>
       <c r="L25" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D26">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E26">
         <v>163</v>
@@ -1471,36 +1465,36 @@
         <v>56</v>
       </c>
       <c r="G26" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="H26" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="I26" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="J26" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="K26">
-        <v>91231233</v>
+        <v>663082682</v>
       </c>
       <c r="L26" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D27">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E27">
         <v>163</v>
@@ -1509,36 +1503,36 @@
         <v>56</v>
       </c>
       <c r="G27" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="H27" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="I27" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="J27" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="K27">
-        <v>91231233</v>
+        <v>663082682</v>
       </c>
       <c r="L27" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C28" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D28">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E28">
         <v>163</v>
@@ -1547,36 +1541,36 @@
         <v>56</v>
       </c>
       <c r="G28" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="H28" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="I28" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="J28" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="K28">
-        <v>91231233</v>
+        <v>663082682</v>
       </c>
       <c r="L28" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C29" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D29">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E29">
         <v>163</v>
@@ -1585,36 +1579,36 @@
         <v>56</v>
       </c>
       <c r="G29" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="H29" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="I29" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="J29" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="K29">
-        <v>91231233</v>
+        <v>663082682</v>
       </c>
       <c r="L29" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B30" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C30" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D30">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E30">
         <v>163</v>
@@ -1623,36 +1617,36 @@
         <v>56</v>
       </c>
       <c r="G30" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="H30" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="I30" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="J30" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="K30">
-        <v>91231233</v>
+        <v>663082682</v>
       </c>
       <c r="L30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B31" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C31" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D31">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E31">
         <v>163</v>
@@ -1661,36 +1655,36 @@
         <v>56</v>
       </c>
       <c r="G31" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="H31" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="I31" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="J31" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="K31">
-        <v>91231233</v>
+        <v>663082682</v>
       </c>
       <c r="L31" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B32" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C32" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D32">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E32">
         <v>163</v>
@@ -1699,36 +1693,36 @@
         <v>56</v>
       </c>
       <c r="G32" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="H32" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="I32" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="J32" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="K32">
-        <v>91231233</v>
+        <v>663082682</v>
       </c>
       <c r="L32" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B33" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C33" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D33">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E33">
         <v>163</v>
@@ -1737,36 +1731,36 @@
         <v>56</v>
       </c>
       <c r="G33" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="H33" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="I33" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="J33" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="K33">
-        <v>91231233</v>
+        <v>663082682</v>
       </c>
       <c r="L33" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B34" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C34" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D34">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E34">
         <v>163</v>
@@ -1775,36 +1769,36 @@
         <v>56</v>
       </c>
       <c r="G34" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="H34" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="I34" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="J34" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="K34">
-        <v>91231233</v>
+        <v>663082682</v>
       </c>
       <c r="L34" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B35" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C35" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D35">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E35">
         <v>163</v>
@@ -1813,36 +1807,36 @@
         <v>56</v>
       </c>
       <c r="G35" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="H35" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="I35" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="J35" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="K35">
-        <v>91231233</v>
+        <v>663082682</v>
       </c>
       <c r="L35" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B36" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C36" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D36">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E36">
         <v>163</v>
@@ -1851,36 +1845,36 @@
         <v>56</v>
       </c>
       <c r="G36" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="H36" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="I36" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="J36" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="K36">
-        <v>91231233</v>
+        <v>663082682</v>
       </c>
       <c r="L36" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B37" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C37" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D37">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E37">
         <v>163</v>
@@ -1889,22 +1883,22 @@
         <v>56</v>
       </c>
       <c r="G37" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="H37" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="I37" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="J37" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="K37">
-        <v>91231233</v>
+        <v>663082682</v>
       </c>
       <c r="L37" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -1942,7 +1936,7 @@
         <v>91231233</v>
       </c>
       <c r="L38" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -1980,7 +1974,7 @@
         <v>91231233</v>
       </c>
       <c r="L39" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -2056,7 +2050,7 @@
         <v>91231233</v>
       </c>
       <c r="L41" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
@@ -2094,21 +2088,21 @@
         <v>91231233</v>
       </c>
       <c r="L42" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B43" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C43" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D43">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E43">
         <v>163</v>
@@ -2117,74 +2111,74 @@
         <v>56</v>
       </c>
       <c r="G43" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="H43" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="I43" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="J43" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="K43">
-        <v>91231233</v>
+        <v>663082682</v>
       </c>
       <c r="L43" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B44" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C44" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D44">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E44">
-        <v>198</v>
+        <v>163</v>
       </c>
       <c r="F44">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="G44" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H44" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="I44" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J44" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="K44">
-        <v>9869515589</v>
+        <v>663082682</v>
       </c>
       <c r="L44" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B45" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C45" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D45">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E45">
         <v>163</v>
@@ -2193,19 +2187,19 @@
         <v>56</v>
       </c>
       <c r="G45" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="H45" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="I45" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="J45" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="K45">
-        <v>91231233</v>
+        <v>663082682</v>
       </c>
       <c r="L45" t="s">
         <v>19</v>
@@ -2213,16 +2207,16 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B46" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C46" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D46">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E46">
         <v>163</v>
@@ -2231,60 +2225,1314 @@
         <v>56</v>
       </c>
       <c r="G46" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="H46" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="I46" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="J46" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="K46">
-        <v>91231233</v>
+        <v>663082682</v>
       </c>
       <c r="L46" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>24</v>
+      </c>
+      <c r="B47" t="s">
+        <v>25</v>
+      </c>
+      <c r="C47" t="s">
+        <v>26</v>
+      </c>
+      <c r="D47">
+        <v>20</v>
+      </c>
+      <c r="E47">
+        <v>163</v>
+      </c>
+      <c r="F47">
+        <v>56</v>
+      </c>
+      <c r="G47" t="s">
+        <v>27</v>
+      </c>
+      <c r="H47" t="s">
+        <v>28</v>
+      </c>
+      <c r="I47" t="s">
+        <v>29</v>
+      </c>
+      <c r="J47" t="s">
+        <v>30</v>
+      </c>
+      <c r="K47">
+        <v>663082682</v>
+      </c>
+      <c r="L47" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>24</v>
+      </c>
+      <c r="B48" t="s">
+        <v>25</v>
+      </c>
+      <c r="C48" t="s">
+        <v>26</v>
+      </c>
+      <c r="D48">
+        <v>20</v>
+      </c>
+      <c r="E48">
+        <v>163</v>
+      </c>
+      <c r="F48">
+        <v>56</v>
+      </c>
+      <c r="G48" t="s">
+        <v>27</v>
+      </c>
+      <c r="H48" t="s">
+        <v>28</v>
+      </c>
+      <c r="I48" t="s">
+        <v>29</v>
+      </c>
+      <c r="J48" t="s">
+        <v>30</v>
+      </c>
+      <c r="K48">
+        <v>663082682</v>
+      </c>
+      <c r="L48" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>24</v>
+      </c>
+      <c r="B49" t="s">
+        <v>25</v>
+      </c>
+      <c r="C49" t="s">
+        <v>26</v>
+      </c>
+      <c r="D49">
+        <v>20</v>
+      </c>
+      <c r="E49">
+        <v>163</v>
+      </c>
+      <c r="F49">
+        <v>56</v>
+      </c>
+      <c r="G49" t="s">
+        <v>27</v>
+      </c>
+      <c r="H49" t="s">
+        <v>28</v>
+      </c>
+      <c r="I49" t="s">
+        <v>29</v>
+      </c>
+      <c r="J49" t="s">
+        <v>30</v>
+      </c>
+      <c r="K49">
+        <v>663082682</v>
+      </c>
+      <c r="L49" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>12</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B50" t="s">
         <v>13</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C50" t="s">
         <v>14</v>
       </c>
-      <c r="D47">
-        <v>18</v>
-      </c>
-      <c r="E47">
-        <v>163</v>
-      </c>
-      <c r="F47">
-        <v>56</v>
-      </c>
-      <c r="G47" t="s">
+      <c r="D50">
+        <v>18</v>
+      </c>
+      <c r="E50">
+        <v>163</v>
+      </c>
+      <c r="F50">
+        <v>56</v>
+      </c>
+      <c r="G50" t="s">
         <v>15</v>
       </c>
-      <c r="H47" t="s">
-        <v>16</v>
-      </c>
-      <c r="I47" t="s">
+      <c r="H50" t="s">
+        <v>16</v>
+      </c>
+      <c r="I50" t="s">
         <v>17</v>
       </c>
-      <c r="J47" t="s">
-        <v>18</v>
-      </c>
-      <c r="K47">
+      <c r="J50" t="s">
+        <v>18</v>
+      </c>
+      <c r="K50">
         <v>91231233</v>
       </c>
-      <c r="L47" t="s">
-        <v>30</v>
+      <c r="L50" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>12</v>
+      </c>
+      <c r="B51" t="s">
+        <v>13</v>
+      </c>
+      <c r="C51" t="s">
+        <v>14</v>
+      </c>
+      <c r="D51">
+        <v>18</v>
+      </c>
+      <c r="E51">
+        <v>163</v>
+      </c>
+      <c r="F51">
+        <v>56</v>
+      </c>
+      <c r="G51" t="s">
+        <v>15</v>
+      </c>
+      <c r="H51" t="s">
+        <v>16</v>
+      </c>
+      <c r="I51" t="s">
+        <v>17</v>
+      </c>
+      <c r="J51" t="s">
+        <v>18</v>
+      </c>
+      <c r="K51">
+        <v>91231233</v>
+      </c>
+      <c r="L51" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>12</v>
+      </c>
+      <c r="B52" t="s">
+        <v>13</v>
+      </c>
+      <c r="C52" t="s">
+        <v>14</v>
+      </c>
+      <c r="D52">
+        <v>18</v>
+      </c>
+      <c r="E52">
+        <v>163</v>
+      </c>
+      <c r="F52">
+        <v>56</v>
+      </c>
+      <c r="G52" t="s">
+        <v>15</v>
+      </c>
+      <c r="H52" t="s">
+        <v>16</v>
+      </c>
+      <c r="I52" t="s">
+        <v>17</v>
+      </c>
+      <c r="J52" t="s">
+        <v>18</v>
+      </c>
+      <c r="K52">
+        <v>91231233</v>
+      </c>
+      <c r="L52" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>12</v>
+      </c>
+      <c r="B53" t="s">
+        <v>13</v>
+      </c>
+      <c r="C53" t="s">
+        <v>14</v>
+      </c>
+      <c r="D53">
+        <v>18</v>
+      </c>
+      <c r="E53">
+        <v>163</v>
+      </c>
+      <c r="F53">
+        <v>56</v>
+      </c>
+      <c r="G53" t="s">
+        <v>15</v>
+      </c>
+      <c r="H53" t="s">
+        <v>16</v>
+      </c>
+      <c r="I53" t="s">
+        <v>17</v>
+      </c>
+      <c r="J53" t="s">
+        <v>18</v>
+      </c>
+      <c r="K53">
+        <v>91231233</v>
+      </c>
+      <c r="L53" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>12</v>
+      </c>
+      <c r="B54" t="s">
+        <v>13</v>
+      </c>
+      <c r="C54" t="s">
+        <v>14</v>
+      </c>
+      <c r="D54">
+        <v>18</v>
+      </c>
+      <c r="E54">
+        <v>163</v>
+      </c>
+      <c r="F54">
+        <v>56</v>
+      </c>
+      <c r="G54" t="s">
+        <v>15</v>
+      </c>
+      <c r="H54" t="s">
+        <v>16</v>
+      </c>
+      <c r="I54" t="s">
+        <v>17</v>
+      </c>
+      <c r="J54" t="s">
+        <v>18</v>
+      </c>
+      <c r="K54">
+        <v>91231233</v>
+      </c>
+      <c r="L54" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>24</v>
+      </c>
+      <c r="B55" t="s">
+        <v>25</v>
+      </c>
+      <c r="C55" t="s">
+        <v>26</v>
+      </c>
+      <c r="D55">
+        <v>20</v>
+      </c>
+      <c r="E55">
+        <v>163</v>
+      </c>
+      <c r="F55">
+        <v>56</v>
+      </c>
+      <c r="G55" t="s">
+        <v>27</v>
+      </c>
+      <c r="H55" t="s">
+        <v>28</v>
+      </c>
+      <c r="I55" t="s">
+        <v>29</v>
+      </c>
+      <c r="J55" t="s">
+        <v>30</v>
+      </c>
+      <c r="K55">
+        <v>663082682</v>
+      </c>
+      <c r="L55" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>24</v>
+      </c>
+      <c r="B56" t="s">
+        <v>25</v>
+      </c>
+      <c r="C56" t="s">
+        <v>26</v>
+      </c>
+      <c r="D56">
+        <v>20</v>
+      </c>
+      <c r="E56">
+        <v>163</v>
+      </c>
+      <c r="F56">
+        <v>56</v>
+      </c>
+      <c r="G56" t="s">
+        <v>27</v>
+      </c>
+      <c r="H56" t="s">
+        <v>28</v>
+      </c>
+      <c r="I56" t="s">
+        <v>29</v>
+      </c>
+      <c r="J56" t="s">
+        <v>30</v>
+      </c>
+      <c r="K56">
+        <v>663082682</v>
+      </c>
+      <c r="L56" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>24</v>
+      </c>
+      <c r="B57" t="s">
+        <v>25</v>
+      </c>
+      <c r="C57" t="s">
+        <v>26</v>
+      </c>
+      <c r="D57">
+        <v>20</v>
+      </c>
+      <c r="E57">
+        <v>163</v>
+      </c>
+      <c r="F57">
+        <v>56</v>
+      </c>
+      <c r="G57" t="s">
+        <v>27</v>
+      </c>
+      <c r="H57" t="s">
+        <v>28</v>
+      </c>
+      <c r="I57" t="s">
+        <v>29</v>
+      </c>
+      <c r="J57" t="s">
+        <v>30</v>
+      </c>
+      <c r="K57">
+        <v>663082682</v>
+      </c>
+      <c r="L57" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>24</v>
+      </c>
+      <c r="B58" t="s">
+        <v>25</v>
+      </c>
+      <c r="C58" t="s">
+        <v>26</v>
+      </c>
+      <c r="D58">
+        <v>20</v>
+      </c>
+      <c r="E58">
+        <v>163</v>
+      </c>
+      <c r="F58">
+        <v>56</v>
+      </c>
+      <c r="G58" t="s">
+        <v>27</v>
+      </c>
+      <c r="H58" t="s">
+        <v>28</v>
+      </c>
+      <c r="I58" t="s">
+        <v>29</v>
+      </c>
+      <c r="J58" t="s">
+        <v>30</v>
+      </c>
+      <c r="K58">
+        <v>663082682</v>
+      </c>
+      <c r="L58" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>24</v>
+      </c>
+      <c r="B59" t="s">
+        <v>25</v>
+      </c>
+      <c r="C59" t="s">
+        <v>26</v>
+      </c>
+      <c r="D59">
+        <v>20</v>
+      </c>
+      <c r="E59">
+        <v>163</v>
+      </c>
+      <c r="F59">
+        <v>56</v>
+      </c>
+      <c r="G59" t="s">
+        <v>27</v>
+      </c>
+      <c r="H59" t="s">
+        <v>28</v>
+      </c>
+      <c r="I59" t="s">
+        <v>29</v>
+      </c>
+      <c r="J59" t="s">
+        <v>30</v>
+      </c>
+      <c r="K59">
+        <v>663082682</v>
+      </c>
+      <c r="L59" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>24</v>
+      </c>
+      <c r="B60" t="s">
+        <v>25</v>
+      </c>
+      <c r="C60" t="s">
+        <v>26</v>
+      </c>
+      <c r="D60">
+        <v>20</v>
+      </c>
+      <c r="E60">
+        <v>163</v>
+      </c>
+      <c r="F60">
+        <v>56</v>
+      </c>
+      <c r="G60" t="s">
+        <v>27</v>
+      </c>
+      <c r="H60" t="s">
+        <v>28</v>
+      </c>
+      <c r="I60" t="s">
+        <v>29</v>
+      </c>
+      <c r="J60" t="s">
+        <v>30</v>
+      </c>
+      <c r="K60">
+        <v>663082682</v>
+      </c>
+      <c r="L60" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>12</v>
+      </c>
+      <c r="B61" t="s">
+        <v>13</v>
+      </c>
+      <c r="C61" t="s">
+        <v>14</v>
+      </c>
+      <c r="D61">
+        <v>18</v>
+      </c>
+      <c r="E61">
+        <v>163</v>
+      </c>
+      <c r="F61">
+        <v>56</v>
+      </c>
+      <c r="G61" t="s">
+        <v>15</v>
+      </c>
+      <c r="H61" t="s">
+        <v>16</v>
+      </c>
+      <c r="I61" t="s">
+        <v>17</v>
+      </c>
+      <c r="J61" t="s">
+        <v>18</v>
+      </c>
+      <c r="K61">
+        <v>91231233</v>
+      </c>
+      <c r="L61" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>12</v>
+      </c>
+      <c r="B62" t="s">
+        <v>13</v>
+      </c>
+      <c r="C62" t="s">
+        <v>14</v>
+      </c>
+      <c r="D62">
+        <v>18</v>
+      </c>
+      <c r="E62">
+        <v>163</v>
+      </c>
+      <c r="F62">
+        <v>56</v>
+      </c>
+      <c r="G62" t="s">
+        <v>15</v>
+      </c>
+      <c r="H62" t="s">
+        <v>16</v>
+      </c>
+      <c r="I62" t="s">
+        <v>17</v>
+      </c>
+      <c r="J62" t="s">
+        <v>18</v>
+      </c>
+      <c r="K62">
+        <v>91231233</v>
+      </c>
+      <c r="L62" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>12</v>
+      </c>
+      <c r="B63" t="s">
+        <v>13</v>
+      </c>
+      <c r="C63" t="s">
+        <v>14</v>
+      </c>
+      <c r="D63">
+        <v>18</v>
+      </c>
+      <c r="E63">
+        <v>163</v>
+      </c>
+      <c r="F63">
+        <v>56</v>
+      </c>
+      <c r="G63" t="s">
+        <v>15</v>
+      </c>
+      <c r="H63" t="s">
+        <v>16</v>
+      </c>
+      <c r="I63" t="s">
+        <v>17</v>
+      </c>
+      <c r="J63" t="s">
+        <v>18</v>
+      </c>
+      <c r="K63">
+        <v>91231233</v>
+      </c>
+      <c r="L63" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>12</v>
+      </c>
+      <c r="B64" t="s">
+        <v>13</v>
+      </c>
+      <c r="C64" t="s">
+        <v>14</v>
+      </c>
+      <c r="D64">
+        <v>18</v>
+      </c>
+      <c r="E64">
+        <v>163</v>
+      </c>
+      <c r="F64">
+        <v>56</v>
+      </c>
+      <c r="G64" t="s">
+        <v>15</v>
+      </c>
+      <c r="H64" t="s">
+        <v>16</v>
+      </c>
+      <c r="I64" t="s">
+        <v>17</v>
+      </c>
+      <c r="J64" t="s">
+        <v>18</v>
+      </c>
+      <c r="K64">
+        <v>91231233</v>
+      </c>
+      <c r="L64" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>12</v>
+      </c>
+      <c r="B65" t="s">
+        <v>13</v>
+      </c>
+      <c r="C65" t="s">
+        <v>14</v>
+      </c>
+      <c r="D65">
+        <v>18</v>
+      </c>
+      <c r="E65">
+        <v>163</v>
+      </c>
+      <c r="F65">
+        <v>56</v>
+      </c>
+      <c r="G65" t="s">
+        <v>15</v>
+      </c>
+      <c r="H65" t="s">
+        <v>16</v>
+      </c>
+      <c r="I65" t="s">
+        <v>17</v>
+      </c>
+      <c r="J65" t="s">
+        <v>18</v>
+      </c>
+      <c r="K65">
+        <v>91231233</v>
+      </c>
+      <c r="L65" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>31</v>
+      </c>
+      <c r="B66" t="s">
+        <v>32</v>
+      </c>
+      <c r="C66" t="s">
+        <v>33</v>
+      </c>
+      <c r="D66">
+        <v>20</v>
+      </c>
+      <c r="E66">
+        <v>163</v>
+      </c>
+      <c r="F66">
+        <v>62</v>
+      </c>
+      <c r="G66" t="s">
+        <v>27</v>
+      </c>
+      <c r="H66" t="s">
+        <v>16</v>
+      </c>
+      <c r="I66" t="s">
+        <v>34</v>
+      </c>
+      <c r="J66" t="s">
+        <v>30</v>
+      </c>
+      <c r="K66">
+        <v>9137893005</v>
+      </c>
+      <c r="L66" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>31</v>
+      </c>
+      <c r="B67" t="s">
+        <v>32</v>
+      </c>
+      <c r="C67" t="s">
+        <v>33</v>
+      </c>
+      <c r="D67">
+        <v>20</v>
+      </c>
+      <c r="E67">
+        <v>163</v>
+      </c>
+      <c r="F67">
+        <v>62</v>
+      </c>
+      <c r="G67" t="s">
+        <v>27</v>
+      </c>
+      <c r="H67" t="s">
+        <v>16</v>
+      </c>
+      <c r="I67" t="s">
+        <v>34</v>
+      </c>
+      <c r="J67" t="s">
+        <v>30</v>
+      </c>
+      <c r="K67">
+        <v>9137893005</v>
+      </c>
+      <c r="L67" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>31</v>
+      </c>
+      <c r="B68" t="s">
+        <v>32</v>
+      </c>
+      <c r="C68" t="s">
+        <v>33</v>
+      </c>
+      <c r="D68">
+        <v>20</v>
+      </c>
+      <c r="E68">
+        <v>163</v>
+      </c>
+      <c r="F68">
+        <v>62</v>
+      </c>
+      <c r="G68" t="s">
+        <v>27</v>
+      </c>
+      <c r="H68" t="s">
+        <v>16</v>
+      </c>
+      <c r="I68" t="s">
+        <v>34</v>
+      </c>
+      <c r="J68" t="s">
+        <v>30</v>
+      </c>
+      <c r="K68">
+        <v>9137893005</v>
+      </c>
+      <c r="L68" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>31</v>
+      </c>
+      <c r="B69" t="s">
+        <v>32</v>
+      </c>
+      <c r="C69" t="s">
+        <v>33</v>
+      </c>
+      <c r="D69">
+        <v>20</v>
+      </c>
+      <c r="E69">
+        <v>163</v>
+      </c>
+      <c r="F69">
+        <v>62</v>
+      </c>
+      <c r="G69" t="s">
+        <v>27</v>
+      </c>
+      <c r="H69" t="s">
+        <v>16</v>
+      </c>
+      <c r="I69" t="s">
+        <v>34</v>
+      </c>
+      <c r="J69" t="s">
+        <v>30</v>
+      </c>
+      <c r="K69">
+        <v>9137893005</v>
+      </c>
+      <c r="L69" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>31</v>
+      </c>
+      <c r="B70" t="s">
+        <v>32</v>
+      </c>
+      <c r="C70" t="s">
+        <v>33</v>
+      </c>
+      <c r="D70">
+        <v>20</v>
+      </c>
+      <c r="E70">
+        <v>163</v>
+      </c>
+      <c r="F70">
+        <v>62</v>
+      </c>
+      <c r="G70" t="s">
+        <v>27</v>
+      </c>
+      <c r="H70" t="s">
+        <v>16</v>
+      </c>
+      <c r="I70" t="s">
+        <v>34</v>
+      </c>
+      <c r="J70" t="s">
+        <v>30</v>
+      </c>
+      <c r="K70">
+        <v>9137893005</v>
+      </c>
+      <c r="L70" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>31</v>
+      </c>
+      <c r="B71" t="s">
+        <v>32</v>
+      </c>
+      <c r="C71" t="s">
+        <v>33</v>
+      </c>
+      <c r="D71">
+        <v>20</v>
+      </c>
+      <c r="E71">
+        <v>163</v>
+      </c>
+      <c r="F71">
+        <v>62</v>
+      </c>
+      <c r="G71" t="s">
+        <v>27</v>
+      </c>
+      <c r="H71" t="s">
+        <v>16</v>
+      </c>
+      <c r="I71" t="s">
+        <v>34</v>
+      </c>
+      <c r="J71" t="s">
+        <v>30</v>
+      </c>
+      <c r="K71">
+        <v>9137893005</v>
+      </c>
+      <c r="L71" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>31</v>
+      </c>
+      <c r="B72" t="s">
+        <v>32</v>
+      </c>
+      <c r="C72" t="s">
+        <v>33</v>
+      </c>
+      <c r="D72">
+        <v>20</v>
+      </c>
+      <c r="E72">
+        <v>163</v>
+      </c>
+      <c r="F72">
+        <v>62</v>
+      </c>
+      <c r="G72" t="s">
+        <v>27</v>
+      </c>
+      <c r="H72" t="s">
+        <v>16</v>
+      </c>
+      <c r="I72" t="s">
+        <v>34</v>
+      </c>
+      <c r="J72" t="s">
+        <v>30</v>
+      </c>
+      <c r="K72">
+        <v>9137893005</v>
+      </c>
+      <c r="L72" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>31</v>
+      </c>
+      <c r="B73" t="s">
+        <v>32</v>
+      </c>
+      <c r="C73" t="s">
+        <v>33</v>
+      </c>
+      <c r="D73">
+        <v>20</v>
+      </c>
+      <c r="E73">
+        <v>163</v>
+      </c>
+      <c r="F73">
+        <v>62</v>
+      </c>
+      <c r="G73" t="s">
+        <v>27</v>
+      </c>
+      <c r="H73" t="s">
+        <v>16</v>
+      </c>
+      <c r="I73" t="s">
+        <v>34</v>
+      </c>
+      <c r="J73" t="s">
+        <v>30</v>
+      </c>
+      <c r="K73">
+        <v>9137893005</v>
+      </c>
+      <c r="L73" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>31</v>
+      </c>
+      <c r="B74" t="s">
+        <v>32</v>
+      </c>
+      <c r="C74" t="s">
+        <v>33</v>
+      </c>
+      <c r="D74">
+        <v>20</v>
+      </c>
+      <c r="E74">
+        <v>163</v>
+      </c>
+      <c r="F74">
+        <v>62</v>
+      </c>
+      <c r="G74" t="s">
+        <v>27</v>
+      </c>
+      <c r="H74" t="s">
+        <v>16</v>
+      </c>
+      <c r="I74" t="s">
+        <v>34</v>
+      </c>
+      <c r="J74" t="s">
+        <v>30</v>
+      </c>
+      <c r="K74">
+        <v>9137893005</v>
+      </c>
+      <c r="L74" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>31</v>
+      </c>
+      <c r="B75" t="s">
+        <v>32</v>
+      </c>
+      <c r="C75" t="s">
+        <v>33</v>
+      </c>
+      <c r="D75">
+        <v>20</v>
+      </c>
+      <c r="E75">
+        <v>163</v>
+      </c>
+      <c r="F75">
+        <v>62</v>
+      </c>
+      <c r="G75" t="s">
+        <v>27</v>
+      </c>
+      <c r="H75" t="s">
+        <v>16</v>
+      </c>
+      <c r="I75" t="s">
+        <v>34</v>
+      </c>
+      <c r="J75" t="s">
+        <v>30</v>
+      </c>
+      <c r="K75">
+        <v>9137893005</v>
+      </c>
+      <c r="L75" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>31</v>
+      </c>
+      <c r="B76" t="s">
+        <v>32</v>
+      </c>
+      <c r="C76" t="s">
+        <v>33</v>
+      </c>
+      <c r="D76">
+        <v>20</v>
+      </c>
+      <c r="E76">
+        <v>163</v>
+      </c>
+      <c r="F76">
+        <v>62</v>
+      </c>
+      <c r="G76" t="s">
+        <v>27</v>
+      </c>
+      <c r="H76" t="s">
+        <v>16</v>
+      </c>
+      <c r="I76" t="s">
+        <v>34</v>
+      </c>
+      <c r="J76" t="s">
+        <v>30</v>
+      </c>
+      <c r="K76">
+        <v>9137893005</v>
+      </c>
+      <c r="L76" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>31</v>
+      </c>
+      <c r="B77" t="s">
+        <v>32</v>
+      </c>
+      <c r="C77" t="s">
+        <v>33</v>
+      </c>
+      <c r="D77">
+        <v>20</v>
+      </c>
+      <c r="E77">
+        <v>163</v>
+      </c>
+      <c r="F77">
+        <v>62</v>
+      </c>
+      <c r="G77" t="s">
+        <v>27</v>
+      </c>
+      <c r="H77" t="s">
+        <v>16</v>
+      </c>
+      <c r="I77" t="s">
+        <v>34</v>
+      </c>
+      <c r="J77" t="s">
+        <v>30</v>
+      </c>
+      <c r="K77">
+        <v>9137893005</v>
+      </c>
+      <c r="L77" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>31</v>
+      </c>
+      <c r="B78" t="s">
+        <v>32</v>
+      </c>
+      <c r="C78" t="s">
+        <v>33</v>
+      </c>
+      <c r="D78">
+        <v>20</v>
+      </c>
+      <c r="E78">
+        <v>163</v>
+      </c>
+      <c r="F78">
+        <v>62</v>
+      </c>
+      <c r="G78" t="s">
+        <v>27</v>
+      </c>
+      <c r="H78" t="s">
+        <v>16</v>
+      </c>
+      <c r="I78" t="s">
+        <v>34</v>
+      </c>
+      <c r="J78" t="s">
+        <v>30</v>
+      </c>
+      <c r="K78">
+        <v>9137893005</v>
+      </c>
+      <c r="L78" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>31</v>
+      </c>
+      <c r="B79" t="s">
+        <v>32</v>
+      </c>
+      <c r="C79" t="s">
+        <v>33</v>
+      </c>
+      <c r="D79">
+        <v>20</v>
+      </c>
+      <c r="E79">
+        <v>163</v>
+      </c>
+      <c r="F79">
+        <v>62</v>
+      </c>
+      <c r="G79" t="s">
+        <v>27</v>
+      </c>
+      <c r="H79" t="s">
+        <v>16</v>
+      </c>
+      <c r="I79" t="s">
+        <v>34</v>
+      </c>
+      <c r="J79" t="s">
+        <v>30</v>
+      </c>
+      <c r="K79">
+        <v>9137893005</v>
+      </c>
+      <c r="L79" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>31</v>
+      </c>
+      <c r="B80" t="s">
+        <v>32</v>
+      </c>
+      <c r="C80" t="s">
+        <v>33</v>
+      </c>
+      <c r="D80">
+        <v>20</v>
+      </c>
+      <c r="E80">
+        <v>163</v>
+      </c>
+      <c r="F80">
+        <v>62</v>
+      </c>
+      <c r="G80" t="s">
+        <v>27</v>
+      </c>
+      <c r="H80" t="s">
+        <v>16</v>
+      </c>
+      <c r="I80" t="s">
+        <v>34</v>
+      </c>
+      <c r="J80" t="s">
+        <v>30</v>
+      </c>
+      <c r="K80">
+        <v>9137893005</v>
+      </c>
+      <c r="L80" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>